<commit_message>
Y03S02: Computer Systems: Coursework 01: fix table naming in Excel solution sheets
</commit_message>
<xml_diff>
--- a/y03s02/computer-systems/coursework/01-solution/data-klokun/y03s02-compsys-coursework-01-klokun.xlsx
+++ b/y03s02/computer-systems/coursework/01-solution/data-klokun/y03s02-compsys-coursework-01-klokun.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/myownreality/university/university-stuff/y03s02/computer-systems/coursework/01-solution/data-klokun/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Files\My Documents\university\y03s02\computer-systems\coursework\01-solution\data-klokun\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="454"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16005" tabRatio="454"/>
   </bookViews>
   <sheets>
     <sheet name="Данные" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -94,37 +94,37 @@
     <t xml:space="preserve">   </t>
   </si>
   <si>
-    <t>Середні значення  1-36</t>
-  </si>
-  <si>
-    <t>Середні значення  37-72</t>
-  </si>
-  <si>
-    <t>Середні значення  73-108</t>
-  </si>
-  <si>
-    <t>Оцінка значення топологічних характеристик  1-36</t>
-  </si>
-  <si>
-    <t>Оцінка значення топологічних характеристик  37-72</t>
-  </si>
-  <si>
-    <t>Оцінка значення топологічних характеристик 73-108</t>
-  </si>
-  <si>
     <t>Сер.діаметр</t>
   </si>
   <si>
-    <t>1-36</t>
+    <t>Дельта оптимального трафика</t>
   </si>
   <si>
-    <t>37-72</t>
+    <t>Середні значення  1-32</t>
   </si>
   <si>
-    <t>73-108</t>
+    <t>Середні значення  33-64</t>
   </si>
   <si>
-    <t>Дельта оптимального трафика</t>
+    <t>Середні значення  65-104</t>
+  </si>
+  <si>
+    <t>Оцінка значення топологічних характеристик  1-32</t>
+  </si>
+  <si>
+    <t>Оцінка значення топологічних характеристик  33-64</t>
+  </si>
+  <si>
+    <t>Оцінка значення топологічних характеристик 65-104</t>
+  </si>
+  <si>
+    <t>1-32</t>
+  </si>
+  <si>
+    <t>33-64</t>
+  </si>
+  <si>
+    <t>65-104</t>
   </si>
 </sst>
 </file>
@@ -345,6 +345,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -360,6 +369,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -369,29 +381,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Гиперссылка" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Открывавшаяся гиперссылка" xfId="2" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -400,7 +403,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -420,8 +423,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.162291169451074"/>
           <c:y val="0.102273105591211"/>
-          <c:w val="0.541766109785203"/>
-          <c:h val="0.628790204745963"/>
+          <c:w val="0.54176610978520301"/>
+          <c:h val="0.62879020474596303"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -471,43 +474,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72.0</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88.0</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>96.0</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>104.0</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -519,43 +522,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -606,43 +609,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72.0</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88.0</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>96.0</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>104.0</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -654,43 +657,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -741,43 +744,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72.0</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88.0</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>96.0</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>104.0</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -789,43 +792,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -866,43 +869,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72.0</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88.0</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>96.0</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>104.0</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -914,43 +917,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -967,11 +970,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2147396864"/>
-        <c:axId val="-2145738320"/>
+        <c:axId val="-931087824"/>
+        <c:axId val="-931094352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2147396864"/>
+        <c:axId val="-931087824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1005,7 +1008,7 @@
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
               <c:x val="0.245823272090989"/>
-              <c:y val="0.852276044028528"/>
+              <c:y val="0.85227604402852797"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1042,10 +1045,10 @@
                 <a:cs typeface="Arial Cyr"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2145738320"/>
+        <c:crossAx val="-931094352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1055,7 +1058,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2145738320"/>
+        <c:axId val="-931094352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1098,8 +1101,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0381861378438806"/>
-              <c:y val="0.272728422036251"/>
+              <c:x val="3.8186137843880599E-2"/>
+              <c:y val="0.27272842203625097"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1136,13 +1139,13 @@
                 <a:cs typeface="Arial Cyr"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2147396864"/>
+        <c:crossAx val="-931087824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="2.0"/>
+        <c:majorUnit val="2"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -1162,10 +1165,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.74352418630947"/>
-          <c:y val="0.164388621337993"/>
-          <c:w val="0.209711949984722"/>
-          <c:h val="0.226034354339741"/>
+          <c:x val="0.74352418630947004"/>
+          <c:y val="0.16438862133799301"/>
+          <c:w val="0.20971194998472201"/>
+          <c:h val="0.22603435433974101"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1194,7 +1197,7 @@
               <a:cs typeface="Arial Cyr"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1227,12 +1230,12 @@
           <a:cs typeface="Arial Cyr"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1241,7 +1244,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1259,10 +1262,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.206185826486271"/>
-          <c:y val="0.0981133883280298"/>
-          <c:w val="0.497423306398128"/>
-          <c:h val="0.641510615990964"/>
+          <c:x val="0.20618582648627101"/>
+          <c:y val="9.8113388328029794E-2"/>
+          <c:w val="0.49742330639812798"/>
+          <c:h val="0.64151061599096404"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1312,43 +1315,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72.0</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88.0</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>96.0</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>104.0</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1363,40 +1366,40 @@
                   <c:v>1.28571428571428</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.06666666666666</c:v>
+                  <c:v>2.0666666666666602</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.53623188405797</c:v>
+                  <c:v>2.5362318840579698</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.93548387096774</c:v>
+                  <c:v>2.9354838709677402</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.3076923076923</c:v>
+                  <c:v>3.3076923076922999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.66666666666666</c:v>
+                  <c:v>3.6666666666666599</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.01818181818181</c:v>
+                  <c:v>4.0181818181818096</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.36507936507936</c:v>
+                  <c:v>4.3650793650793602</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.70892018779342</c:v>
+                  <c:v>4.7089201877934199</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>5.0506329113924</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.39080459770114</c:v>
+                  <c:v>5.3908045977011403</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.7298245614035</c:v>
+                  <c:v>5.7298245614035004</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.06796116504854</c:v>
+                  <c:v>6.0679611650485397</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1447,43 +1450,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72.0</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88.0</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>96.0</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>104.0</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1498,19 +1501,19 @@
                   <c:v>1.28571428571428</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.06666666666666</c:v>
+                  <c:v>2.0666666666666602</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.53623188405797</c:v>
+                  <c:v>2.5362318840579698</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.80645161290322</c:v>
+                  <c:v>2.8064516129032202</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.97948717948717</c:v>
+                  <c:v>2.9794871794871698</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.09929078014184</c:v>
+                  <c:v>3.0992907801418399</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>3.18701298701298</c:v>
@@ -1519,19 +1522,19 @@
                   <c:v>3.25396825396825</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.30672926447574</c:v>
+                  <c:v>3.3067292644757398</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.34936708860759</c:v>
+                  <c:v>3.3493670886075901</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.38453500522466</c:v>
+                  <c:v>3.3845350052246599</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.41403508771929</c:v>
+                  <c:v>3.4140350877192902</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.43913368185212</c:v>
+                  <c:v>3.4391336818521201</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1582,43 +1585,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72.0</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88.0</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>96.0</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>104.0</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1633,40 +1636,40 @@
                   <c:v>1.28571428571428</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.06666666666666</c:v>
+                  <c:v>2.0666666666666602</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.30434782608695</c:v>
+                  <c:v>2.3043478260869499</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.6774193548387</c:v>
+                  <c:v>2.6774193548387002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.89743589743589</c:v>
+                  <c:v>2.8974358974358898</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.2127659574468</c:v>
+                  <c:v>3.2127659574468002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.43636363636363</c:v>
+                  <c:v>3.4363636363636298</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.73015873015873</c:v>
+                  <c:v>3.7301587301587298</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.95774647887323</c:v>
+                  <c:v>3.9577464788732302</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>4.24050632911392</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.47126436781609</c:v>
+                  <c:v>4.4712643678160902</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.74736842105263</c:v>
+                  <c:v>4.7473684210526299</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.98058252427184</c:v>
+                  <c:v>4.9805825242718402</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1707,43 +1710,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72.0</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88.0</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>96.0</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>104.0</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1758,31 +1761,31 @@
                   <c:v>1.28571428571428</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.06666666666666</c:v>
+                  <c:v>2.0666666666666602</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.53623188405797</c:v>
+                  <c:v>2.5362318840579698</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.6774193548387</c:v>
+                  <c:v>2.6774193548387002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.97948717948717</c:v>
+                  <c:v>2.9794871794871698</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.09929078014184</c:v>
+                  <c:v>3.0992907801418399</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.35324675324675</c:v>
+                  <c:v>3.3532467532467498</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.41269841269841</c:v>
+                  <c:v>3.4126984126984099</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.50704225352112</c:v>
+                  <c:v>3.5070422535211199</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.71392405063291</c:v>
+                  <c:v>3.7139240506329099</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>3.78578892371995</c:v>
@@ -1791,7 +1794,7 @@
                   <c:v>3.87719298245614</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.06049290515309</c:v>
+                  <c:v>4.0604929051530902</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1808,11 +1811,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2145634784"/>
-        <c:axId val="-2145629136"/>
+        <c:axId val="-931103056"/>
+        <c:axId val="-966138464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2145634784"/>
+        <c:axId val="-931103056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1845,8 +1848,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.270618904595688"/>
-              <c:y val="0.85660542432196"/>
+              <c:x val="0.27061890459568799"/>
+              <c:y val="0.85660542432195996"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1883,10 +1886,10 @@
                 <a:cs typeface="Arial Cyr"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2145629136"/>
+        <c:crossAx val="-966138464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1896,7 +1899,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2145629136"/>
+        <c:axId val="-966138464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1939,8 +1942,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0541237499951681"/>
-              <c:y val="0.26415135608049"/>
+              <c:x val="5.4123749995168099E-2"/>
+              <c:y val="0.26415135608049001"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1977,13 +1980,13 @@
                 <a:cs typeface="Arial Cyr"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2145634784"/>
+        <c:crossAx val="-931103056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="2.0"/>
+        <c:majorUnit val="2"/>
       </c:valAx>
       <c:spPr>
         <a:solidFill>
@@ -2003,10 +2006,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.745224313704228"/>
+          <c:x val="0.74522431370422804"/>
           <c:y val="0.20748970219019"/>
           <c:w val="0.200704440458984"/>
-          <c:h val="0.227898525356438"/>
+          <c:h val="0.22789852535643801"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2035,7 +2038,7 @@
               <a:cs typeface="Arial Cyr"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2068,12 +2071,12 @@
           <a:cs typeface="Arial Cyr"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2082,7 +2085,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2102,8 +2105,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.112359550561798"/>
           <c:y val="0.106463878326996"/>
-          <c:w val="0.56661316211878"/>
-          <c:h val="0.5893536121673"/>
+          <c:w val="0.56661316211877999"/>
+          <c:h val="0.58935361216729998"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2153,43 +2156,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72.0</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88.0</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>96.0</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>104.0</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2201,43 +2204,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2288,43 +2291,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72.0</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88.0</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>96.0</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>104.0</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2336,43 +2339,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>17.0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18.0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>19.0</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2423,43 +2426,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72.0</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88.0</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>96.0</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>104.0</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2471,43 +2474,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2548,43 +2551,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72.0</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88.0</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>96.0</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>104.0</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2596,43 +2599,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2649,11 +2652,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2145573984"/>
-        <c:axId val="-2145568352"/>
+        <c:axId val="-750780832"/>
+        <c:axId val="-750781376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2145573984"/>
+        <c:axId val="-750780832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2724,10 +2727,10 @@
                 <a:cs typeface="Arial Cyr"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2145568352"/>
+        <c:crossAx val="-750781376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2737,7 +2740,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2145568352"/>
+        <c:axId val="-750781376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2780,8 +2783,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0256821699296196"/>
-              <c:y val="0.327485074728353"/>
+              <c:x val="2.5682169929619601E-2"/>
+              <c:y val="0.32748507472835298"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2818,10 +2821,10 @@
                 <a:cs typeface="Arial Cyr"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2145573984"/>
+        <c:crossAx val="-750780832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2844,7 +2847,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.7091442169469"/>
-          <c:y val="0.261025590095011"/>
+          <c:y val="0.26102559009501097"/>
           <c:w val="0.227201545235415"/>
           <c:h val="0.254245704637998"/>
         </c:manualLayout>
@@ -2875,7 +2878,7 @@
               <a:cs typeface="Arial Cyr"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2908,12 +2911,12 @@
           <a:cs typeface="Arial Cyr"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2922,7 +2925,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2941,9 +2944,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.153846394616378"/>
-          <c:y val="0.106060998390885"/>
-          <c:w val="0.525641848272624"/>
-          <c:h val="0.590911276749219"/>
+          <c:y val="0.10606099839088499"/>
+          <c:w val="0.52564184827262395"/>
+          <c:h val="0.59091127674921895"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -2993,43 +2996,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72.0</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88.0</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>96.0</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>104.0</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3041,43 +3044,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41.0</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>62.0</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>83.0</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>104.0</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>125.0</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>146.0</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>167.0</c:v>
+                  <c:v>167</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>188.0</c:v>
+                  <c:v>188</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>209.0</c:v>
+                  <c:v>209</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>230.0</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>251.0</c:v>
+                  <c:v>251</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>272.0</c:v>
+                  <c:v>272</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3137,43 +3140,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72.0</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88.0</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>96.0</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>104.0</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3185,43 +3188,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41.0</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>62.0</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>83.0</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>104.0</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>125.0</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>146.0</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>167.0</c:v>
+                  <c:v>167</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>188.0</c:v>
+                  <c:v>188</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>209.0</c:v>
+                  <c:v>209</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>230.0</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>251.0</c:v>
+                  <c:v>251</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>272.0</c:v>
+                  <c:v>272</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3272,43 +3275,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72.0</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88.0</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>96.0</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>104.0</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3320,43 +3323,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41.0</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>63.0</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>84.0</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>105.0</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>126.0</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>147.0</c:v>
+                  <c:v>147</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>168.0</c:v>
+                  <c:v>168</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>189.0</c:v>
+                  <c:v>189</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>210.0</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>231.0</c:v>
+                  <c:v>231</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>252.0</c:v>
+                  <c:v>252</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>273.0</c:v>
+                  <c:v>273</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3397,43 +3400,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72.0</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88.0</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>96.0</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>104.0</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3445,43 +3448,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41.0</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>62.0</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>84.0</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>105.0</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>127.0</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>148.0</c:v>
+                  <c:v>148</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>170.0</c:v>
+                  <c:v>170</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>192.0</c:v>
+                  <c:v>192</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>213.0</c:v>
+                  <c:v>213</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>235.0</c:v>
+                  <c:v>235</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>257.0</c:v>
+                  <c:v>257</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>278.0</c:v>
+                  <c:v>278</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3498,11 +3501,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2145511808"/>
-        <c:axId val="-2145506176"/>
+        <c:axId val="-750779744"/>
+        <c:axId val="-750778112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2145511808"/>
+        <c:axId val="-750779744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3535,8 +3538,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.277244022579369"/>
-              <c:y val="0.833336453098401"/>
+              <c:x val="0.27724402257936898"/>
+              <c:y val="0.83333645309840099"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -3573,10 +3576,10 @@
                 <a:cs typeface="Arial Cyr"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2145506176"/>
+        <c:crossAx val="-750778112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3586,7 +3589,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2145506176"/>
+        <c:axId val="-750778112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3629,7 +3632,7 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0256409592636537"/>
+              <c:x val="2.5640959263653701E-2"/>
               <c:y val="0.2"/>
             </c:manualLayout>
           </c:layout>
@@ -3667,10 +3670,10 @@
                 <a:cs typeface="Arial Cyr"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2145511808"/>
+        <c:crossAx val="-750779744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3692,10 +3695,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.706975306859483"/>
-          <c:y val="0.263522438577299"/>
-          <c:w val="0.216894063696937"/>
-          <c:h val="0.239872988961387"/>
+          <c:x val="0.70697530685948295"/>
+          <c:y val="0.26352243857729901"/>
+          <c:w val="0.21689406369693701"/>
+          <c:h val="0.23987298896138701"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3724,7 +3727,7 @@
               <a:cs typeface="Arial Cyr"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3757,12 +3760,12 @@
           <a:cs typeface="Arial Cyr"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3771,7 +3774,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3791,7 +3794,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.132800103750081"/>
           <c:y val="0.105660572045571"/>
-          <c:w val="0.547200427500334"/>
+          <c:w val="0.54720042750033404"/>
           <c:h val="0.592453921826949"/>
         </c:manualLayout>
       </c:layout>
@@ -3842,43 +3845,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72.0</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88.0</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>96.0</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>104.0</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3893,34 +3896,34 @@
                   <c:v>0.36734693877551</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.516666666666666</c:v>
+                  <c:v>0.51666666666666605</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.563607085346215</c:v>
+                  <c:v>0.56360708534621495</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.652329749103942</c:v>
+                  <c:v>0.65232974910394204</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.735042735042735</c:v>
+                  <c:v>0.73504273504273498</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.814814814814814</c:v>
+                  <c:v>0.81481481481481399</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.892929292929293</c:v>
+                  <c:v>0.89292929292929302</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.970017636684303</c:v>
+                  <c:v>0.97001763668430296</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.04642670839853</c:v>
+                  <c:v>1.0464267083985299</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.12236286919831</c:v>
+                  <c:v>1.1223628691983101</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.19795657726692</c:v>
+                  <c:v>1.1979565772669201</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1.27329434697855</c:v>
@@ -3977,43 +3980,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72.0</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88.0</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>96.0</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>104.0</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4028,40 +4031,40 @@
                   <c:v>0.36734693877551</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.516666666666666</c:v>
+                  <c:v>0.51666666666666605</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.563607085346215</c:v>
+                  <c:v>0.56360708534621495</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.561290322580645</c:v>
+                  <c:v>0.56129032258064504</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.541724941724941</c:v>
+                  <c:v>0.54172494172494101</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.516548463356974</c:v>
+                  <c:v>0.51654846335697402</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.49030969030969</c:v>
+                  <c:v>0.49030969030969002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.46485260770975</c:v>
+                  <c:v>0.46485260770975001</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.440897235263432</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.418670886075949</c:v>
+                  <c:v>0.41867088607594899</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.39818058884996</c:v>
+                  <c:v>0.39818058884995999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.37933723196881</c:v>
+                  <c:v>0.37933723196880997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.362014071773908</c:v>
+                  <c:v>0.36201407177390799</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4112,43 +4115,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64.0</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>72.0</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>88.0</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>96.0</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>104.0</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4163,40 +4166,40 @@
                   <c:v>0.36734693877551</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.516666666666666</c:v>
+                  <c:v>0.51666666666666605</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.51207729468599</c:v>
+                  <c:v>0.51207729468598995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.594982078853046</c:v>
+                  <c:v>0.59498207885304599</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.643874643874643</c:v>
+                  <c:v>0.64387464387464299</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.713947990543735</c:v>
+                  <c:v>0.71394799054373503</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.763636363636363</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.828924162257495</c:v>
+                  <c:v>0.82892416225749499</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.879499217527386</c:v>
+                  <c:v>0.87949921752738602</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.942334739803094</c:v>
+                  <c:v>0.94233473980309401</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.993614303959131</c:v>
+                  <c:v>0.99361430395913097</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1.05497076023391</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.10679611650485</c:v>
+                  <c:v>1.1067961165048501</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4240,40 +4243,40 @@
                   <c:v>0.36734693877551</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.516666666666666</c:v>
+                  <c:v>0.51666666666666605</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.563607085346215</c:v>
+                  <c:v>0.56360708534621495</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.594982078853046</c:v>
+                  <c:v>0.59498207885304599</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.595897435897435</c:v>
+                  <c:v>0.59589743589743505</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.619858156028368</c:v>
+                  <c:v>0.61985815602836802</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.67064935064935</c:v>
+                  <c:v>0.67064935064935005</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.62049062049062</c:v>
+                  <c:v>0.62049062049061998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.63764404609475</c:v>
+                  <c:v>0.63764404609475001</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.675258918296893</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.688325258858174</c:v>
+                  <c:v>0.68832525885817397</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.704944178628389</c:v>
+                  <c:v>0.70494417862838898</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.738271437300563</c:v>
+                  <c:v>0.73827143730056299</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4290,11 +4293,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2145452688"/>
-        <c:axId val="-2145447056"/>
+        <c:axId val="-750783552"/>
+        <c:axId val="-750784640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2145452688"/>
+        <c:axId val="-750783552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4327,7 +4330,7 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.267200117684404"/>
+              <c:x val="0.26720011768440399"/>
               <c:y val="0.833964062184535"/>
             </c:manualLayout>
           </c:layout>
@@ -4365,10 +4368,10 @@
                 <a:cs typeface="Arial Cyr"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2145447056"/>
+        <c:crossAx val="-750784640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4378,7 +4381,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2145447056"/>
+        <c:axId val="-750784640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4421,7 +4424,7 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0256000743269923"/>
+              <c:x val="2.5600074326992302E-2"/>
               <c:y val="0.2"/>
             </c:manualLayout>
           </c:layout>
@@ -4459,10 +4462,10 @@
                 <a:cs typeface="Arial Cyr"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2145452688"/>
+        <c:crossAx val="-750783552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4479,10 +4482,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.708207108400646"/>
-          <c:y val="0.267567212809552"/>
-          <c:w val="0.233103344724836"/>
-          <c:h val="0.237465901368477"/>
+          <c:x val="0.70820710840064605"/>
+          <c:y val="0.26756721280955198"/>
+          <c:w val="0.23310334472483599"/>
+          <c:h val="0.23746590136847701"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -4511,7 +4514,7 @@
               <a:cs typeface="Arial Cyr"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="ru-RU"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4544,12 +4547,12 @@
           <a:cs typeface="Arial Cyr"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="ru-RU"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4986,103 +4989,103 @@
   <dimension ref="A1:AC95"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="G26" zoomScale="106" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+      <selection activeCell="S44" sqref="S44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" customWidth="1"/>
-    <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="13.5" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="19.83203125" customWidth="1"/>
-    <col min="8" max="8" width="25.5" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" customWidth="1"/>
-    <col min="11" max="11" width="14.83203125" customWidth="1"/>
-    <col min="15" max="15" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
+    <col min="15" max="15" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="26"/>
-      <c r="H1" s="24" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="29"/>
+      <c r="H1" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="26"/>
-      <c r="O1" s="24" t="s">
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="29"/>
+      <c r="O1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="26"/>
-      <c r="V1" s="24" t="s">
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="29"/>
+      <c r="V1" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="25"/>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="26"/>
-    </row>
-    <row r="2" spans="1:27" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="29"/>
+    </row>
+    <row r="2" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="26"/>
-      <c r="H2" s="27" t="s">
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="29"/>
+      <c r="H2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="24" t="s">
+      <c r="I2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="26"/>
-      <c r="O2" s="27" t="s">
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="29"/>
+      <c r="O2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="24" t="s">
+      <c r="P2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="T2" s="26"/>
-      <c r="V2" s="27" t="s">
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="29"/>
+      <c r="V2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="24" t="s">
+      <c r="W2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="25"/>
-      <c r="Z2" s="25"/>
-      <c r="AA2" s="26"/>
-    </row>
-    <row r="3" spans="1:27" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="28"/>
+      <c r="X2" s="28"/>
+      <c r="Y2" s="28"/>
+      <c r="Z2" s="28"/>
+      <c r="AA2" s="29"/>
+    </row>
+    <row r="3" spans="1:27" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="31"/>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
@@ -5098,7 +5101,7 @@
       <c r="F3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="35"/>
+      <c r="H3" s="32"/>
       <c r="I3" s="2" t="s">
         <v>3</v>
       </c>
@@ -5114,7 +5117,7 @@
       <c r="M3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="28"/>
+      <c r="O3" s="31"/>
       <c r="P3" s="2" t="s">
         <v>3</v>
       </c>
@@ -5130,7 +5133,7 @@
       <c r="T3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="V3" s="28"/>
+      <c r="V3" s="31"/>
       <c r="W3" s="2" t="s">
         <v>3</v>
       </c>
@@ -5147,7 +5150,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>8</v>
       </c>
@@ -5221,7 +5224,7 @@
         <v>0.36734693877551</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>16</v>
       </c>
@@ -5295,7 +5298,7 @@
         <v>0.51666666666666605</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>24</v>
       </c>
@@ -5369,7 +5372,7 @@
         <v>0.56360708534621495</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>32</v>
       </c>
@@ -5443,7 +5446,7 @@
         <v>0.59498207885304599</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>40</v>
       </c>
@@ -5517,7 +5520,7 @@
         <v>0.59589743589743505</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>48</v>
       </c>
@@ -5591,7 +5594,7 @@
         <v>0.61985815602836802</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>56</v>
       </c>
@@ -5665,7 +5668,7 @@
         <v>0.67064935064935005</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>64</v>
       </c>
@@ -5739,7 +5742,7 @@
         <v>0.62049062049061998</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>72</v>
       </c>
@@ -5813,7 +5816,7 @@
         <v>0.63764404609475001</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>80</v>
       </c>
@@ -5887,7 +5890,7 @@
         <v>0.675258918296893</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>88</v>
       </c>
@@ -5961,7 +5964,7 @@
         <v>0.68832525885817397</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>96</v>
       </c>
@@ -6035,7 +6038,7 @@
         <v>0.70494417862838898</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>104</v>
       </c>
@@ -6109,13 +6112,13 @@
         <v>0.73827143730056299</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="F17"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="F18"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="1"/>
@@ -6123,106 +6126,106 @@
       <c r="E19" s="1"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="5"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="5"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" s="5"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="5"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="5"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A30" s="5"/>
       <c r="W30" s="11"/>
       <c r="Z30" s="11"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="W31" s="11"/>
       <c r="Z31" s="11"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="W32" s="11"/>
       <c r="Z32" s="11"/>
     </row>
-    <row r="33" spans="2:29" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:29" x14ac:dyDescent="0.2">
       <c r="W33" s="11"/>
       <c r="Z33" s="11"/>
     </row>
-    <row r="34" spans="2:29" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:29" x14ac:dyDescent="0.2">
       <c r="W34" s="11"/>
       <c r="Z34" s="11"/>
     </row>
-    <row r="35" spans="2:29" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:29" x14ac:dyDescent="0.2">
       <c r="W35" s="11"/>
       <c r="Z35" s="11"/>
       <c r="AB35" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="2:29" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:29" x14ac:dyDescent="0.2">
       <c r="W36" s="11"/>
       <c r="Z36" s="11"/>
     </row>
-    <row r="40" spans="2:29" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:29" x14ac:dyDescent="0.2">
       <c r="R40" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="2:29" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="2:29" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
-      <c r="I42" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="J42" s="29"/>
-      <c r="K42" s="29"/>
-      <c r="L42" s="29"/>
-      <c r="M42" s="29"/>
-      <c r="N42" s="29"/>
-      <c r="P42" s="30" t="s">
+    <row r="41" spans="2:29" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="2:29" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" s="33"/>
+      <c r="D42" s="33"/>
+      <c r="E42" s="33"/>
+      <c r="F42" s="33"/>
+      <c r="G42" s="33"/>
+      <c r="I42" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="J42" s="33"/>
+      <c r="K42" s="33"/>
+      <c r="L42" s="33"/>
+      <c r="M42" s="33"/>
+      <c r="N42" s="33"/>
+      <c r="P42" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="Q42" s="32" t="s">
+      <c r="Q42" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="R42" s="33"/>
-      <c r="S42" s="34"/>
+      <c r="R42" s="25"/>
+      <c r="S42" s="26"/>
       <c r="T42" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="2:29" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:29" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B43" s="7" t="s">
         <v>10</v>
       </c>
@@ -6230,7 +6233,7 @@
         <v>3</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>11</v>
@@ -6242,7 +6245,7 @@
         <v>7</v>
       </c>
       <c r="H43" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="I43" s="7" t="s">
         <v>10</v>
@@ -6251,7 +6254,7 @@
         <v>3</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="L43" s="8" t="s">
         <v>11</v>
@@ -6262,21 +6265,21 @@
       <c r="N43" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="P43" s="31"/>
+      <c r="P43" s="35"/>
       <c r="Q43" s="21" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R43" s="22" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="S43" s="23" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T43" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="2:29" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:29" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B44" s="7" t="s">
         <v>12</v>
       </c>
@@ -6342,7 +6345,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="2:29" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:29" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B45" s="7" t="s">
         <v>13</v>
       </c>
@@ -6408,7 +6411,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="2:29" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:29" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B46" s="7" t="s">
         <v>14</v>
       </c>
@@ -6477,7 +6480,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="2:29" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:29" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B47" s="16" t="s">
         <v>18</v>
       </c>
@@ -6543,28 +6546,28 @@
         <v>52</v>
       </c>
     </row>
-    <row r="48" spans="2:29" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="C48" s="29"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="29"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="29"/>
-      <c r="I48" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="J48" s="29"/>
-      <c r="K48" s="29"/>
-      <c r="L48" s="29"/>
-      <c r="M48" s="29"/>
-      <c r="N48" s="29"/>
+    <row r="48" spans="2:29" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" s="33"/>
+      <c r="D48" s="33"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="33"/>
+      <c r="I48" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="J48" s="33"/>
+      <c r="K48" s="33"/>
+      <c r="L48" s="33"/>
+      <c r="M48" s="33"/>
+      <c r="N48" s="33"/>
       <c r="AA48" s="13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="2:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B49" s="7" t="s">
         <v>10</v>
       </c>
@@ -6572,7 +6575,7 @@
         <v>3</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E49" s="8" t="s">
         <v>11</v>
@@ -6590,7 +6593,7 @@
         <v>3</v>
       </c>
       <c r="K49" s="8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="L49" s="8" t="s">
         <v>11</v>
@@ -6602,7 +6605,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="2:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B50" s="7" t="s">
         <v>12</v>
       </c>
@@ -6649,7 +6652,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="2:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B51" s="7" t="s">
         <v>13</v>
       </c>
@@ -6696,7 +6699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B52" s="7" t="s">
         <v>14</v>
       </c>
@@ -6743,7 +6746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="2:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B53" s="16" t="s">
         <v>18</v>
       </c>
@@ -6790,25 +6793,25 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="2:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="C54" s="29"/>
-      <c r="D54" s="29"/>
-      <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="29"/>
-      <c r="I54" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="J54" s="29"/>
-      <c r="K54" s="29"/>
-      <c r="L54" s="29"/>
-      <c r="M54" s="29"/>
-      <c r="N54" s="29"/>
-    </row>
-    <row r="55" spans="2:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C54" s="33"/>
+      <c r="D54" s="33"/>
+      <c r="E54" s="33"/>
+      <c r="F54" s="33"/>
+      <c r="G54" s="33"/>
+      <c r="I54" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="J54" s="33"/>
+      <c r="K54" s="33"/>
+      <c r="L54" s="33"/>
+      <c r="M54" s="33"/>
+      <c r="N54" s="33"/>
+    </row>
+    <row r="55" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B55" s="7" t="s">
         <v>10</v>
       </c>
@@ -6816,7 +6819,7 @@
         <v>3</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>11</v>
@@ -6834,7 +6837,7 @@
         <v>3</v>
       </c>
       <c r="K55" s="8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="L55" s="8" t="s">
         <v>11</v>
@@ -6846,7 +6849,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="2:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B56" s="7" t="s">
         <v>12</v>
       </c>
@@ -6893,7 +6896,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="2:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B57" s="7" t="s">
         <v>13</v>
       </c>
@@ -6940,7 +6943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="2:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B58" s="7" t="s">
         <v>14</v>
       </c>
@@ -6987,7 +6990,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="2:14" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B59" s="16" t="s">
         <v>18</v>
       </c>
@@ -7034,113 +7037,126 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="60" spans="2:14" x14ac:dyDescent="0.2">
       <c r="F60"/>
     </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="61" spans="2:14" x14ac:dyDescent="0.2">
       <c r="F61"/>
     </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="62" spans="2:14" x14ac:dyDescent="0.2">
       <c r="F62"/>
     </row>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="63" spans="2:14" x14ac:dyDescent="0.2">
       <c r="F63"/>
     </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="64" spans="2:14" x14ac:dyDescent="0.2">
       <c r="F64"/>
     </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="65" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F65"/>
     </row>
-    <row r="66" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="66" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F66"/>
     </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="67" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F67"/>
     </row>
-    <row r="68" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="68" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F68"/>
     </row>
-    <row r="69" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="69" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F69"/>
     </row>
-    <row r="70" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="70" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F70"/>
     </row>
-    <row r="71" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="71" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F71"/>
     </row>
-    <row r="72" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="72" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F72"/>
     </row>
-    <row r="73" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="73" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F73"/>
     </row>
-    <row r="74" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="74" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F74"/>
     </row>
-    <row r="75" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="75" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F75"/>
     </row>
-    <row r="76" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="76" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F76"/>
     </row>
-    <row r="77" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="77" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F77"/>
     </row>
-    <row r="79" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="79" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F79"/>
     </row>
-    <row r="80" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="80" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F80"/>
     </row>
-    <row r="81" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="81" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F81"/>
     </row>
-    <row r="82" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="82" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F82"/>
     </row>
-    <row r="83" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="83" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F83"/>
     </row>
-    <row r="84" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="84" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F84"/>
     </row>
-    <row r="85" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="85" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F85"/>
     </row>
-    <row r="86" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="86" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F86"/>
     </row>
-    <row r="87" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="87" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F87"/>
     </row>
-    <row r="88" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="88" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F88"/>
     </row>
-    <row r="89" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="89" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F89"/>
     </row>
-    <row r="90" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="90" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F90"/>
     </row>
-    <row r="91" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="91" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F91"/>
     </row>
-    <row r="92" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="92" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F92"/>
     </row>
-    <row r="93" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="93" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F93"/>
     </row>
-    <row r="94" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="94" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F94"/>
     </row>
-    <row r="95" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="95" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F95"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="V1:AA1"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="W2:AA2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="I48:N48"/>
+    <mergeCell ref="I54:N54"/>
+    <mergeCell ref="P42:P43"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="I42:N42"/>
     <mergeCell ref="Q42:S42"/>
     <mergeCell ref="O1:T1"/>
     <mergeCell ref="O2:O3"/>
@@ -7148,19 +7164,6 @@
     <mergeCell ref="H1:M1"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:M2"/>
-    <mergeCell ref="I48:N48"/>
-    <mergeCell ref="I54:N54"/>
-    <mergeCell ref="P42:P43"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="B54:G54"/>
-    <mergeCell ref="I42:N42"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="V1:AA1"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="W2:AA2"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:F2"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -7175,9 +7178,9 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -7191,7 +7194,7 @@
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>